<commit_message>
Só ajuste de conteudo de exemplo
</commit_message>
<xml_diff>
--- a/contatos.xlsx
+++ b/contatos.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Atila\XVRI\Projetos Proprios\Agenda_Excell_Celular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DDB3E9-59C5-4DE7-8244-8331412E9370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F101C313-5930-42E7-B4A9-CD074E9B1D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="contatos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -54,22 +54,22 @@
     <t>XVRI</t>
   </si>
   <si>
-    <t>atila.xavier@gmail.com</t>
-  </si>
-  <si>
     <t>Bruno XX</t>
   </si>
   <si>
-    <t>021981135356</t>
-  </si>
-  <si>
-    <t>021999747208</t>
-  </si>
-  <si>
     <t>021912345678</t>
   </si>
   <si>
     <t>bb.xx@aol.com</t>
+  </si>
+  <si>
+    <t>021981130000</t>
+  </si>
+  <si>
+    <t>021999747200</t>
+  </si>
+  <si>
+    <t>atila.xx@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,29 +441,29 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>